<commit_message>
added rount to template
</commit_message>
<xml_diff>
--- a/test/templates/with-diagram.xlsx
+++ b/test/templates/with-diagram.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27311"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A768C5F-0E59-41C1-A8AD-61529641B71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08697BAA-4377-4FDF-841C-4F73730E8325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
     <t>End</t>
   </si>
   <si>
-    <t>Duration</t>
+    <t>Duration, days</t>
   </si>
   <si>
     <t>Cost per hour, $/h</t>
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1991,7 +1991,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="3" t="e">
-        <f>SUM(G17:G17)</f>
+        <f>ROUND(SUM(G17:G17), 2)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2007,14 +2007,14 @@
         <v>28</v>
       </c>
       <c r="E17" s="15" t="e">
-        <f>D17-C17</f>
+        <f>ROUND(D17-C17, 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="F17" s="16">
         <v>10</v>
       </c>
       <c r="G17" s="16" t="e">
-        <f>E17*F17*24</f>
+        <f>ROUND(E17*F17*24, 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="H17" s="3"/>
@@ -2037,14 +2037,14 @@
         <v>29</v>
       </c>
       <c r="E19" s="18" t="e">
-        <f>SUM(E16:E18)</f>
+        <f>ROUND(SUM(E16:E18), 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>30</v>
       </c>
       <c r="G19" s="20" t="e">
-        <f>SUM(G16:G18)</f>
+        <f>ROUND(SUM(G16:G18), 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="H19" s="26"/>

</xml_diff>